<commit_message>
adds visit type during import
</commit_message>
<xml_diff>
--- a/custom/samveg/tests/case_importer/data/missing_values_rch_case_upload.xlsx
+++ b/custom/samveg/tests/case_importer/data/missing_values_rch_case_upload.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">Rch_id</t>
   </si>
@@ -35,9 +35,6 @@
   </si>
   <si>
     <t xml:space="preserve">Health_Block</t>
-  </si>
-  <si>
-    <t xml:space="preserve">visit_type</t>
   </si>
   <si>
     <t xml:space="preserve">owner_name</t>
@@ -156,13 +153,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1:H2"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -171,45 +171,42 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>9999999999</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>8</v>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>98765</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="F3" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>